<commit_message>
Add uuids to test data (pulled from #93)
Signed-off-by: James Noss <jnoss@jhu.edu>
</commit_message>
<xml_diff>
--- a/biospecdb/apps/uploader/tests/data/meta_data.xlsx
+++ b/biospecdb/apps/uploader/tests/data/meta_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamienoss/repos/biospecdb-project/biospecdb/biospecdb/apps/uploader/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AC09807-4069-FD42-954C-0EB259C6670F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3D27FC2-3146-3D44-9A2F-36D2D029CA72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="1000" windowWidth="25040" windowHeight="14400" xr2:uid="{6C67B765-75CA-5F42-88FE-D1F4BED05A15}"/>
+    <workbookView xWindow="21620" yWindow="2860" windowWidth="15040" windowHeight="14400" xr2:uid="{6C67B765-75CA-5F42-88FE-D1F4BED05A15}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="58">
   <si>
     <t>Patient ID</t>
   </si>
@@ -180,6 +180,36 @@
   </si>
   <si>
     <t>Days of Symptoms onset</t>
+  </si>
+  <si>
+    <t>fd39991e-8791-4a17-91de-5fee78236d6d</t>
+  </si>
+  <si>
+    <t>f52d82f3-1fb4-4734-b0d3-56665153243c</t>
+  </si>
+  <si>
+    <t>d0ffda4a-6e60-4bff-8929-1c5b998c8d28</t>
+  </si>
+  <si>
+    <t>d0e2eef7-2fc2-41c1-b1a9-226a9686772d</t>
+  </si>
+  <si>
+    <t>e7defaff-ac0d-409d-a497-cebe94c4ce01</t>
+  </si>
+  <si>
+    <t>2c8e8f01-7e2b-4ff6-9be6-60fa4914cd24</t>
+  </si>
+  <si>
+    <t>2204c553-1098-42e6-87cd-8baeedfed672</t>
+  </si>
+  <si>
+    <t>651bb92d-74af-44d2-a3ca-ef3cbc70ee0c</t>
+  </si>
+  <si>
+    <t>34c9a874-1227-44d2-9274-3ff757e0fcff</t>
+  </si>
+  <si>
+    <t>4fd057b7-7078-4900-825c-28d145afa25e</t>
   </si>
 </sst>
 </file>
@@ -268,10 +298,10 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -602,162 +632,165 @@
   <dimension ref="A1:AJ12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G2"/>
+      <selection activeCell="A3" sqref="A3:A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="46.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="N1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="O1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="P1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="Q1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="R1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="S1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="T1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="U1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="V1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="W1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="X1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="Y1" s="4" t="s">
+      <c r="Y1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" s="4" t="s">
+      <c r="Z1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AA1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AB1" s="3" t="s">
+      <c r="AB1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="AC1" s="3" t="s">
+      <c r="AC1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="AD1" s="3" t="s">
+      <c r="AD1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AE1" s="3" t="s">
+      <c r="AE1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="AF1" s="3" t="s">
+      <c r="AF1" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="AG1" s="3" t="s">
+      <c r="AG1" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="AH1" s="3" t="s">
+      <c r="AH1" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="AI1" s="3" t="s">
+      <c r="AI1" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="AJ1" s="3" t="s">
+      <c r="AJ1" s="4" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A2" s="3"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="4"/>
-      <c r="R2" s="4"/>
-      <c r="S2" s="4"/>
-      <c r="T2" s="4"/>
-      <c r="U2" s="4"/>
-      <c r="V2" s="3"/>
-      <c r="W2" s="4"/>
-      <c r="X2" s="4"/>
-      <c r="Y2" s="4"/>
-      <c r="Z2" s="4"/>
-      <c r="AA2" s="3"/>
-      <c r="AB2" s="3"/>
-      <c r="AC2" s="3"/>
-      <c r="AD2" s="3"/>
-      <c r="AE2" s="3"/>
-      <c r="AF2" s="3"/>
-      <c r="AG2" s="3"/>
-      <c r="AH2" s="3"/>
-      <c r="AI2" s="3"/>
-      <c r="AJ2" s="3"/>
+      <c r="A2" s="4"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="4"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="3"/>
+      <c r="AA2" s="4"/>
+      <c r="AB2" s="4"/>
+      <c r="AC2" s="4"/>
+      <c r="AD2" s="4"/>
+      <c r="AE2" s="4"/>
+      <c r="AF2" s="4"/>
+      <c r="AG2" s="4"/>
+      <c r="AH2" s="4"/>
+      <c r="AI2" s="4"/>
+      <c r="AJ2" s="4"/>
     </row>
     <row r="3" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
-        <v>1</v>
+      <c r="A3" s="1" t="s">
+        <v>48</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>35</v>
@@ -854,8 +887,8 @@
       <c r="AJ3" s="1"/>
     </row>
     <row r="4" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
-        <v>2</v>
+      <c r="A4" s="1" t="s">
+        <v>49</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>35</v>
@@ -952,8 +985,8 @@
       <c r="AJ4" s="1"/>
     </row>
     <row r="5" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
-        <v>3</v>
+      <c r="A5" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>35</v>
@@ -1050,8 +1083,8 @@
       <c r="AJ5" s="1"/>
     </row>
     <row r="6" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
-        <v>4</v>
+      <c r="A6" s="1" t="s">
+        <v>51</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>35</v>
@@ -1148,8 +1181,8 @@
       <c r="AJ6" s="1"/>
     </row>
     <row r="7" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A7" s="1">
-        <v>5</v>
+      <c r="A7" s="1" t="s">
+        <v>52</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>35</v>
@@ -1246,8 +1279,8 @@
       <c r="AJ7" s="1"/>
     </row>
     <row r="8" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A8" s="1">
-        <v>6</v>
+      <c r="A8" s="1" t="s">
+        <v>53</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>46</v>
@@ -1348,8 +1381,8 @@
       <c r="AJ8" s="1"/>
     </row>
     <row r="9" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A9" s="1">
-        <v>7</v>
+      <c r="A9" s="1" t="s">
+        <v>54</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>46</v>
@@ -1450,8 +1483,8 @@
       <c r="AJ9" s="1"/>
     </row>
     <row r="10" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A10" s="1">
-        <v>8</v>
+      <c r="A10" s="1" t="s">
+        <v>55</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>35</v>
@@ -1548,8 +1581,8 @@
       <c r="AJ10" s="1"/>
     </row>
     <row r="11" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A11" s="1">
-        <v>9</v>
+      <c r="A11" s="1" t="s">
+        <v>56</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>35</v>
@@ -1646,8 +1679,8 @@
       <c r="AJ11" s="1"/>
     </row>
     <row r="12" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A12" s="1">
-        <v>10</v>
+      <c r="A12" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>35</v>
@@ -1745,6 +1778,30 @@
     </row>
   </sheetData>
   <mergeCells count="36">
+    <mergeCell ref="AJ1:AJ2"/>
+    <mergeCell ref="Y1:Y2"/>
+    <mergeCell ref="Z1:Z2"/>
+    <mergeCell ref="AA1:AA2"/>
+    <mergeCell ref="AB1:AB2"/>
+    <mergeCell ref="AC1:AC2"/>
+    <mergeCell ref="AD1:AD2"/>
+    <mergeCell ref="AE1:AE2"/>
+    <mergeCell ref="AF1:AF2"/>
+    <mergeCell ref="AG1:AG2"/>
+    <mergeCell ref="AH1:AH2"/>
+    <mergeCell ref="AI1:AI2"/>
+    <mergeCell ref="X1:X2"/>
+    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="N1:N2"/>
+    <mergeCell ref="O1:O2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="Q1:Q2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="V1:V2"/>
+    <mergeCell ref="W1:W2"/>
     <mergeCell ref="L1:L2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
@@ -1757,30 +1814,6 @@
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="K1:K2"/>
-    <mergeCell ref="X1:X2"/>
-    <mergeCell ref="M1:M2"/>
-    <mergeCell ref="N1:N2"/>
-    <mergeCell ref="O1:O2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="Q1:Q2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="V1:V2"/>
-    <mergeCell ref="W1:W2"/>
-    <mergeCell ref="AJ1:AJ2"/>
-    <mergeCell ref="Y1:Y2"/>
-    <mergeCell ref="Z1:Z2"/>
-    <mergeCell ref="AA1:AA2"/>
-    <mergeCell ref="AB1:AB2"/>
-    <mergeCell ref="AC1:AC2"/>
-    <mergeCell ref="AD1:AD2"/>
-    <mergeCell ref="AE1:AE2"/>
-    <mergeCell ref="AF1:AF2"/>
-    <mergeCell ref="AG1:AG2"/>
-    <mergeCell ref="AH1:AH2"/>
-    <mergeCell ref="AI1:AI2"/>
   </mergeCells>
   <conditionalFormatting sqref="H3:U12">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">

</xml_diff>

<commit_message>
Revert back the "Gender" column name
</commit_message>
<xml_diff>
--- a/biospecdb/apps/uploader/tests/data/meta_data.xlsx
+++ b/biospecdb/apps/uploader/tests/data/meta_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vkluzner/Work/git/BSR/biospecdb/biospecdb/apps/uploader/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F8A2694-F1A4-2241-A2EF-D670C3540CB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E581F4A5-41CA-5C44-B14C-40E630467E0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="21620" yWindow="2860" windowWidth="15040" windowHeight="14400" xr2:uid="{6C67B765-75CA-5F42-88FE-D1F4BED05A15}"/>
   </bookViews>
@@ -209,10 +209,10 @@
     <t>4fd057b7-7078-4900-825c-28d145afa25e</t>
   </si>
   <si>
-    <t>Gender (X/M/F)</t>
-  </si>
-  <si>
     <t>X</t>
+  </si>
+  <si>
+    <t>Gender (M/F)</t>
   </si>
 </sst>
 </file>
@@ -301,10 +301,10 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -635,7 +635,7 @@
   <dimension ref="A1:AJ12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="E1" sqref="E1:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -644,152 +644,152 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="F1" s="4" t="s">
+      <c r="E1" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="N1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="O1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="P1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="Q1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="R1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="S1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="T1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="U1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="V1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="W1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="X1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="Y1" s="4" t="s">
+      <c r="Y1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="Z1" s="4" t="s">
+      <c r="Z1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AA1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="AB1" s="3" t="s">
+      <c r="AB1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AC1" s="3" t="s">
+      <c r="AC1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="AD1" s="3" t="s">
+      <c r="AD1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="AE1" s="3" t="s">
+      <c r="AE1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AF1" s="3" t="s">
+      <c r="AF1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="AG1" s="3" t="s">
+      <c r="AG1" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="AH1" s="3" t="s">
+      <c r="AH1" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="AI1" s="3" t="s">
+      <c r="AI1" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="AJ1" s="3" t="s">
+      <c r="AJ1" s="4" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A2" s="3"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="4"/>
-      <c r="R2" s="4"/>
-      <c r="S2" s="4"/>
-      <c r="T2" s="4"/>
-      <c r="U2" s="4"/>
-      <c r="V2" s="3"/>
-      <c r="W2" s="4"/>
-      <c r="X2" s="4"/>
-      <c r="Y2" s="4"/>
-      <c r="Z2" s="4"/>
-      <c r="AA2" s="3"/>
-      <c r="AB2" s="3"/>
-      <c r="AC2" s="3"/>
-      <c r="AD2" s="3"/>
-      <c r="AE2" s="3"/>
-      <c r="AF2" s="3"/>
-      <c r="AG2" s="3"/>
-      <c r="AH2" s="3"/>
-      <c r="AI2" s="3"/>
-      <c r="AJ2" s="3"/>
+      <c r="A2" s="4"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="4"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="3"/>
+      <c r="AA2" s="4"/>
+      <c r="AB2" s="4"/>
+      <c r="AC2" s="4"/>
+      <c r="AD2" s="4"/>
+      <c r="AE2" s="4"/>
+      <c r="AF2" s="4"/>
+      <c r="AG2" s="4"/>
+      <c r="AH2" s="4"/>
+      <c r="AI2" s="4"/>
+      <c r="AJ2" s="4"/>
     </row>
     <row r="3" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
@@ -1691,7 +1691,7 @@
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F12" s="1">
         <v>31</v>
@@ -1781,6 +1781,30 @@
     </row>
   </sheetData>
   <mergeCells count="36">
+    <mergeCell ref="AJ1:AJ2"/>
+    <mergeCell ref="Y1:Y2"/>
+    <mergeCell ref="Z1:Z2"/>
+    <mergeCell ref="AA1:AA2"/>
+    <mergeCell ref="AB1:AB2"/>
+    <mergeCell ref="AC1:AC2"/>
+    <mergeCell ref="AD1:AD2"/>
+    <mergeCell ref="AE1:AE2"/>
+    <mergeCell ref="AF1:AF2"/>
+    <mergeCell ref="AG1:AG2"/>
+    <mergeCell ref="AH1:AH2"/>
+    <mergeCell ref="AI1:AI2"/>
+    <mergeCell ref="X1:X2"/>
+    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="N1:N2"/>
+    <mergeCell ref="O1:O2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="Q1:Q2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="V1:V2"/>
+    <mergeCell ref="W1:W2"/>
     <mergeCell ref="L1:L2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
@@ -1793,30 +1817,6 @@
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="K1:K2"/>
-    <mergeCell ref="X1:X2"/>
-    <mergeCell ref="M1:M2"/>
-    <mergeCell ref="N1:N2"/>
-    <mergeCell ref="O1:O2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="Q1:Q2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="V1:V2"/>
-    <mergeCell ref="W1:W2"/>
-    <mergeCell ref="AJ1:AJ2"/>
-    <mergeCell ref="Y1:Y2"/>
-    <mergeCell ref="Z1:Z2"/>
-    <mergeCell ref="AA1:AA2"/>
-    <mergeCell ref="AB1:AB2"/>
-    <mergeCell ref="AC1:AC2"/>
-    <mergeCell ref="AD1:AD2"/>
-    <mergeCell ref="AE1:AE2"/>
-    <mergeCell ref="AF1:AF2"/>
-    <mergeCell ref="AG1:AG2"/>
-    <mergeCell ref="AH1:AH2"/>
-    <mergeCell ref="AI1:AI2"/>
   </mergeCells>
   <conditionalFormatting sqref="H3:U12">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">

</xml_diff>

<commit_message>
Expand instrument and measurement fields
Signed-off-by: James Noss <jnoss@jhu.edu>
</commit_message>
<xml_diff>
--- a/biospecdb/apps/uploader/tests/data/meta_data.xlsx
+++ b/biospecdb/apps/uploader/tests/data/meta_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vkluzner/Work/git/BSR/biospecdb/biospecdb/apps/uploader/tests/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamienoss/repos/biospecdb-project/biospecdb/biospecdb/apps/uploader/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E581F4A5-41CA-5C44-B14C-40E630467E0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9797CA18-C3E6-2948-A060-95AC7CB09E4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21620" yWindow="2860" windowWidth="15040" windowHeight="14400" xr2:uid="{6C67B765-75CA-5F42-88FE-D1F4BED05A15}"/>
+    <workbookView xWindow="5820" yWindow="3700" windowWidth="15040" windowHeight="14400" xr2:uid="{6C67B765-75CA-5F42-88FE-D1F4BED05A15}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -110,12 +110,6 @@
     <t>CHRONIC OR NEUROMUSCULAR NEUROLOGICAL DISEASE</t>
   </si>
   <si>
-    <t>Spectra Measurement</t>
-  </si>
-  <si>
-    <t>Spectrometer</t>
-  </si>
-  <si>
     <t>ATR Crystal</t>
   </si>
   <si>
@@ -155,9 +149,6 @@
     <t>ATR-FTIR</t>
   </si>
   <si>
-    <t>Agilent Cory 630</t>
-  </si>
-  <si>
     <t>ZnSe</t>
   </si>
   <si>
@@ -213,6 +204,15 @@
   </si>
   <si>
     <t>Gender (M/F)</t>
+  </si>
+  <si>
+    <t>4205d8ac-90c1-4529-90b2-6751f665c403</t>
+  </si>
+  <si>
+    <t>Instrument</t>
+  </si>
+  <si>
+    <t>Measurement type</t>
   </si>
 </sst>
 </file>
@@ -634,8 +634,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFCC409A-0F6A-A445-A77C-A7B22D278FED}">
   <dimension ref="A1:AJ12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E2"/>
+    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
+      <selection activeCell="AA1" sqref="AA1:AA2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -657,13 +657,13 @@
         <v>3</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>5</v>
@@ -723,34 +723,34 @@
         <v>23</v>
       </c>
       <c r="AA1" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="AB1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="AC1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="AB1" s="4" t="s">
+      <c r="AD1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AC1" s="4" t="s">
+      <c r="AE1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="AD1" s="4" t="s">
+      <c r="AF1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="AE1" s="4" t="s">
+      <c r="AG1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AF1" s="4" t="s">
+      <c r="AH1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="AG1" s="4" t="s">
+      <c r="AI1" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="AH1" s="4" t="s">
+      <c r="AJ1" s="4" t="s">
         <v>31</v>
-      </c>
-      <c r="AI1" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="AJ1" s="4" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:36" x14ac:dyDescent="0.2">
@@ -793,15 +793,15 @@
     </row>
     <row r="3" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F3" s="1">
         <v>21</v>
@@ -810,70 +810,70 @@
         <v>7</v>
       </c>
       <c r="H3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AA3" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="I3" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="K3" s="1" t="s">
+      <c r="AB3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC3" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q3" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="S3" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="T3" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="U3" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="V3" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="W3" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="X3" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="Y3" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="Z3" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AA3" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AB3" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AC3" s="1" t="s">
-        <v>40</v>
       </c>
       <c r="AD3" s="1"/>
       <c r="AE3" s="1">
@@ -881,25 +881,25 @@
       </c>
       <c r="AF3" s="1"/>
       <c r="AG3" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="AH3" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="AI3" s="1"/>
       <c r="AJ3" s="1"/>
     </row>
     <row r="4" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F4" s="1">
         <v>97</v>
@@ -908,70 +908,70 @@
         <v>1</v>
       </c>
       <c r="H4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="X4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Z4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AA4" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="I4" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="K4" s="1" t="s">
+      <c r="AB4" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC4" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q4" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="R4" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="S4" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="T4" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="U4" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="V4" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="W4" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="X4" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="Y4" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="Z4" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AA4" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AB4" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AC4" s="1" t="s">
-        <v>40</v>
       </c>
       <c r="AD4" s="1"/>
       <c r="AE4" s="1">
@@ -979,25 +979,25 @@
       </c>
       <c r="AF4" s="1"/>
       <c r="AG4" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="AH4" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="AI4" s="1"/>
       <c r="AJ4" s="1"/>
     </row>
     <row r="5" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F5" s="1">
         <v>6</v>
@@ -1006,70 +1006,70 @@
         <v>2</v>
       </c>
       <c r="H5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="U5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="W5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="X5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Z5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AA5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB5" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC5" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="O5" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="P5" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q5" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="R5" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="S5" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="T5" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="U5" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="V5" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="W5" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="X5" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="Y5" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="Z5" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AA5" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AB5" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AC5" s="1" t="s">
-        <v>40</v>
       </c>
       <c r="AD5" s="1"/>
       <c r="AE5" s="1">
@@ -1077,25 +1077,25 @@
       </c>
       <c r="AF5" s="1"/>
       <c r="AG5" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="AH5" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="AI5" s="1"/>
       <c r="AJ5" s="1"/>
     </row>
     <row r="6" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F6" s="1">
         <v>44</v>
@@ -1104,70 +1104,70 @@
         <v>2</v>
       </c>
       <c r="H6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="T6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="U6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="V6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="W6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="X6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Z6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AA6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB6" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC6" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="O6" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="P6" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q6" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="R6" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="S6" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="T6" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="U6" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="V6" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="W6" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="X6" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="Y6" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="Z6" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AA6" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AB6" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AC6" s="1" t="s">
-        <v>40</v>
       </c>
       <c r="AD6" s="1"/>
       <c r="AE6" s="1">
@@ -1175,25 +1175,25 @@
       </c>
       <c r="AF6" s="1"/>
       <c r="AG6" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="AH6" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="AI6" s="1"/>
       <c r="AJ6" s="1"/>
     </row>
     <row r="7" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F7" s="1">
         <v>55</v>
@@ -1202,70 +1202,70 @@
         <v>3</v>
       </c>
       <c r="H7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="T7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="U7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="V7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="W7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="X7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Z7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AA7" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="I7" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="K7" s="1" t="s">
+      <c r="AB7" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC7" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="N7" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="O7" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="P7" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q7" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="R7" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="S7" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="T7" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="U7" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="V7" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="W7" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="X7" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="Y7" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="Z7" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AA7" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AB7" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AC7" s="1" t="s">
-        <v>40</v>
       </c>
       <c r="AD7" s="1"/>
       <c r="AE7" s="1">
@@ -1273,20 +1273,20 @@
       </c>
       <c r="AF7" s="1"/>
       <c r="AG7" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="AH7" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="AI7" s="1"/>
       <c r="AJ7" s="1"/>
     </row>
     <row r="8" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C8" s="1">
         <v>24.8</v>
@@ -1295,79 +1295,79 @@
         <v>24.8</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F8" s="1">
         <v>22</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="H8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="R8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="S8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="T8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="U8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="V8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="W8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="X8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Z8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AA8" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="I8" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="M8" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="N8" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="O8" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="P8" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q8" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="R8" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="S8" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="T8" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="U8" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="V8" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="W8" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="X8" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="Y8" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="Z8" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AA8" s="1" t="s">
-        <v>38</v>
-      </c>
       <c r="AB8" s="1" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="AC8" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="AD8" s="1"/>
       <c r="AE8" s="1">
@@ -1375,20 +1375,20 @@
       </c>
       <c r="AF8" s="1"/>
       <c r="AG8" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="AH8" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="AI8" s="1"/>
       <c r="AJ8" s="1"/>
     </row>
     <row r="9" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C9" s="1">
         <v>18.18</v>
@@ -1397,7 +1397,7 @@
         <v>18.18</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F9" s="1">
         <v>17</v>
@@ -1406,70 +1406,70 @@
         <v>3</v>
       </c>
       <c r="H9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="R9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="S9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="T9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="U9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="V9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="W9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="X9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Z9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AA9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB9" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC9" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="L9" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="M9" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="N9" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="O9" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="P9" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q9" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="R9" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="S9" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="T9" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="U9" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="V9" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="W9" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="X9" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="Y9" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="Z9" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AA9" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AB9" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AC9" s="1" t="s">
-        <v>40</v>
       </c>
       <c r="AD9" s="1"/>
       <c r="AE9" s="1">
@@ -1477,25 +1477,25 @@
       </c>
       <c r="AF9" s="1"/>
       <c r="AG9" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="AH9" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="AI9" s="1"/>
       <c r="AJ9" s="1"/>
     </row>
     <row r="10" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F10" s="1">
         <v>57</v>
@@ -1504,70 +1504,70 @@
         <v>5</v>
       </c>
       <c r="H10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="R10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="S10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="T10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="U10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="V10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="W10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="X10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Z10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AA10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB10" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC10" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="M10" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="N10" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="O10" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="P10" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q10" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="R10" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="S10" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="T10" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="U10" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="V10" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="W10" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="X10" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="Y10" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="Z10" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AA10" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AB10" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AC10" s="1" t="s">
-        <v>40</v>
       </c>
       <c r="AD10" s="1"/>
       <c r="AE10" s="1">
@@ -1575,25 +1575,25 @@
       </c>
       <c r="AF10" s="1"/>
       <c r="AG10" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="AH10" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="AI10" s="1"/>
       <c r="AJ10" s="1"/>
     </row>
     <row r="11" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F11" s="1">
         <v>9</v>
@@ -1602,70 +1602,70 @@
         <v>11</v>
       </c>
       <c r="H11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="R11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="S11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="T11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="U11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="V11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="W11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="X11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Z11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AA11" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="I11" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="K11" s="1" t="s">
+      <c r="AB11" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC11" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="L11" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="M11" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="N11" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="O11" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="P11" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q11" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="R11" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="S11" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="T11" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="U11" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="V11" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="W11" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="X11" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="Y11" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="Z11" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AA11" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AB11" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AC11" s="1" t="s">
-        <v>40</v>
       </c>
       <c r="AD11" s="1"/>
       <c r="AE11" s="1">
@@ -1673,25 +1673,25 @@
       </c>
       <c r="AF11" s="1"/>
       <c r="AG11" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="AH11" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="AI11" s="1"/>
       <c r="AJ11" s="1"/>
     </row>
     <row r="12" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F12" s="1">
         <v>31</v>
@@ -1700,70 +1700,70 @@
         <v>12</v>
       </c>
       <c r="H12" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="O12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q12" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="R12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="S12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="T12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="U12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="V12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="W12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="X12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Z12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AA12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB12" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC12" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="L12" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="M12" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="N12" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="O12" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="P12" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q12" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="R12" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="S12" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="T12" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="U12" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="V12" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="W12" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="X12" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="Y12" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="Z12" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AA12" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AB12" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AC12" s="1" t="s">
-        <v>40</v>
       </c>
       <c r="AD12" s="1"/>
       <c r="AE12" s="1">
@@ -1771,10 +1771,10 @@
       </c>
       <c r="AF12" s="1"/>
       <c r="AG12" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="AH12" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="AI12" s="1"/>
       <c r="AJ12" s="1"/>

</xml_diff>

<commit_message>
Tweak Observation.days_observed.verbose_name -> 'days observed', not 'days of symptoms onset
Signed-off-by: James Noss <jnoss@jhu.edu>
</commit_message>
<xml_diff>
--- a/biospecdb/apps/uploader/tests/data/meta_data.xlsx
+++ b/biospecdb/apps/uploader/tests/data/meta_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamienoss/repos/biospecdb-project/biospecdb/biospecdb/apps/uploader/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9797CA18-C3E6-2948-A060-95AC7CB09E4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93A31751-27B2-5543-8BB6-226C6777B1EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5820" yWindow="3700" windowWidth="15040" windowHeight="14400" xr2:uid="{6C67B765-75CA-5F42-88FE-D1F4BED05A15}"/>
   </bookViews>
@@ -167,9 +167,6 @@
     <t>Positive</t>
   </si>
   <si>
-    <t>Days of Symptoms onset</t>
-  </si>
-  <si>
     <t>fd39991e-8791-4a17-91de-5fee78236d6d</t>
   </si>
   <si>
@@ -213,6 +210,9 @@
   </si>
   <si>
     <t>Measurement type</t>
+  </si>
+  <si>
+    <t>Days observed</t>
   </si>
 </sst>
 </file>
@@ -301,10 +301,10 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -634,8 +634,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFCC409A-0F6A-A445-A77C-A7B22D278FED}">
   <dimension ref="A1:AJ12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
-      <selection activeCell="AA1" sqref="AA1:AA2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -644,156 +644,156 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="F1" s="3" t="s">
+      <c r="E1" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="H1" s="3" t="s">
+      <c r="G1" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="N1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="O1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="P1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="Q1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="R1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="S1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="T1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="U1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="V1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="W1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="X1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="Y1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="Z1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="AA1" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="AB1" s="4" t="s">
+      <c r="AA1" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="AC1" s="4" t="s">
+      <c r="AB1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="AD1" s="4" t="s">
+      <c r="AD1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="AE1" s="4" t="s">
+      <c r="AE1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="AF1" s="4" t="s">
+      <c r="AF1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="AG1" s="4" t="s">
+      <c r="AG1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="AH1" s="4" t="s">
+      <c r="AH1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="AI1" s="4" t="s">
+      <c r="AI1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="AJ1" s="4" t="s">
+      <c r="AJ1" s="3" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A2" s="4"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="4"/>
-      <c r="Q2" s="3"/>
-      <c r="R2" s="3"/>
-      <c r="S2" s="3"/>
-      <c r="T2" s="3"/>
-      <c r="U2" s="3"/>
-      <c r="V2" s="4"/>
-      <c r="W2" s="3"/>
-      <c r="X2" s="3"/>
-      <c r="Y2" s="3"/>
-      <c r="Z2" s="3"/>
-      <c r="AA2" s="4"/>
-      <c r="AB2" s="4"/>
-      <c r="AC2" s="4"/>
-      <c r="AD2" s="4"/>
-      <c r="AE2" s="4"/>
-      <c r="AF2" s="4"/>
-      <c r="AG2" s="4"/>
-      <c r="AH2" s="4"/>
-      <c r="AI2" s="4"/>
-      <c r="AJ2" s="4"/>
+      <c r="A2" s="3"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="4"/>
+      <c r="R2" s="4"/>
+      <c r="S2" s="4"/>
+      <c r="T2" s="4"/>
+      <c r="U2" s="4"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="4"/>
+      <c r="X2" s="4"/>
+      <c r="Y2" s="4"/>
+      <c r="Z2" s="4"/>
+      <c r="AA2" s="3"/>
+      <c r="AB2" s="3"/>
+      <c r="AC2" s="3"/>
+      <c r="AD2" s="3"/>
+      <c r="AE2" s="3"/>
+      <c r="AF2" s="3"/>
+      <c r="AG2" s="3"/>
+      <c r="AH2" s="3"/>
+      <c r="AI2" s="3"/>
+      <c r="AJ2" s="3"/>
     </row>
     <row r="3" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>32</v>
@@ -870,7 +870,7 @@
         <v>36</v>
       </c>
       <c r="AB3" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="AC3" s="1" t="s">
         <v>37</v>
@@ -891,7 +891,7 @@
     </row>
     <row r="4" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>32</v>
@@ -968,7 +968,7 @@
         <v>36</v>
       </c>
       <c r="AB4" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="AC4" s="1" t="s">
         <v>37</v>
@@ -989,7 +989,7 @@
     </row>
     <row r="5" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>32</v>
@@ -1066,7 +1066,7 @@
         <v>36</v>
       </c>
       <c r="AB5" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="AC5" s="1" t="s">
         <v>37</v>
@@ -1087,7 +1087,7 @@
     </row>
     <row r="6" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>32</v>
@@ -1164,7 +1164,7 @@
         <v>36</v>
       </c>
       <c r="AB6" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="AC6" s="1" t="s">
         <v>37</v>
@@ -1185,7 +1185,7 @@
     </row>
     <row r="7" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>32</v>
@@ -1262,7 +1262,7 @@
         <v>36</v>
       </c>
       <c r="AB7" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="AC7" s="1" t="s">
         <v>37</v>
@@ -1283,7 +1283,7 @@
     </row>
     <row r="8" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>42</v>
@@ -1364,7 +1364,7 @@
         <v>36</v>
       </c>
       <c r="AB8" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="AC8" s="1" t="s">
         <v>37</v>
@@ -1385,7 +1385,7 @@
     </row>
     <row r="9" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>42</v>
@@ -1466,7 +1466,7 @@
         <v>36</v>
       </c>
       <c r="AB9" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="AC9" s="1" t="s">
         <v>37</v>
@@ -1487,7 +1487,7 @@
     </row>
     <row r="10" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>32</v>
@@ -1564,7 +1564,7 @@
         <v>36</v>
       </c>
       <c r="AB10" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="AC10" s="1" t="s">
         <v>37</v>
@@ -1585,7 +1585,7 @@
     </row>
     <row r="11" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>32</v>
@@ -1662,7 +1662,7 @@
         <v>36</v>
       </c>
       <c r="AB11" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="AC11" s="1" t="s">
         <v>37</v>
@@ -1683,7 +1683,7 @@
     </row>
     <row r="12" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>32</v>
@@ -1691,7 +1691,7 @@
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F12" s="1">
         <v>31</v>
@@ -1760,7 +1760,7 @@
         <v>36</v>
       </c>
       <c r="AB12" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="AC12" s="1" t="s">
         <v>37</v>
@@ -1781,6 +1781,30 @@
     </row>
   </sheetData>
   <mergeCells count="36">
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="X1:X2"/>
+    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="N1:N2"/>
+    <mergeCell ref="O1:O2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="Q1:Q2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="V1:V2"/>
+    <mergeCell ref="W1:W2"/>
     <mergeCell ref="AJ1:AJ2"/>
     <mergeCell ref="Y1:Y2"/>
     <mergeCell ref="Z1:Z2"/>
@@ -1793,30 +1817,6 @@
     <mergeCell ref="AG1:AG2"/>
     <mergeCell ref="AH1:AH2"/>
     <mergeCell ref="AI1:AI2"/>
-    <mergeCell ref="X1:X2"/>
-    <mergeCell ref="M1:M2"/>
-    <mergeCell ref="N1:N2"/>
-    <mergeCell ref="O1:O2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="Q1:Q2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="V1:V2"/>
-    <mergeCell ref="W1:W2"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="J1:J2"/>
-    <mergeCell ref="K1:K2"/>
   </mergeCells>
   <conditionalFormatting sqref="H3:U12">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">

</xml_diff>

<commit_message>
Add Observable(name='gender') & Observable.value_choices & Observable.validator
Signed-off-by: James Noss <jnoss@jhu.edu>
</commit_message>
<xml_diff>
--- a/biospecdb/apps/uploader/tests/data/meta_data.xlsx
+++ b/biospecdb/apps/uploader/tests/data/meta_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamienoss/repos/biospecdb-project/biospecdb/biospecdb/apps/uploader/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93A31751-27B2-5543-8BB6-226C6777B1EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F9875CD-4871-FD4A-B7FF-1AFC548AB8E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5820" yWindow="3700" windowWidth="15040" windowHeight="14400" xr2:uid="{6C67B765-75CA-5F42-88FE-D1F4BED05A15}"/>
   </bookViews>
@@ -137,9 +137,6 @@
     <t>Negative</t>
   </si>
   <si>
-    <t>F</t>
-  </si>
-  <si>
     <t>No</t>
   </si>
   <si>
@@ -158,9 +155,6 @@
     <t>None</t>
   </si>
   <si>
-    <t>M</t>
-  </si>
-  <si>
     <t>Unknown</t>
   </si>
   <si>
@@ -197,12 +191,6 @@
     <t>4fd057b7-7078-4900-825c-28d145afa25e</t>
   </si>
   <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>Gender (M/F)</t>
-  </si>
-  <si>
     <t>4205d8ac-90c1-4529-90b2-6751f665c403</t>
   </si>
   <si>
@@ -213,6 +201,18 @@
   </si>
   <si>
     <t>Days observed</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>man</t>
+  </si>
+  <si>
+    <t>woman</t>
+  </si>
+  <si>
+    <t>prefer not to state</t>
   </si>
 </sst>
 </file>
@@ -301,10 +301,10 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -336,9 +336,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -376,7 +376,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -482,7 +482,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -624,7 +624,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -635,7 +635,7 @@
   <dimension ref="A1:AJ12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -644,156 +644,156 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="F1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="N1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="O1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="P1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="Q1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="R1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="S1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="T1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="U1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="V1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="W1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="X1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="Y1" s="4" t="s">
+      <c r="Y1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="Z1" s="4" t="s">
+      <c r="Z1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="AA1" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="AB1" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="AC1" s="3" t="s">
+      <c r="AA1" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB1" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="AC1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="AD1" s="3" t="s">
+      <c r="AD1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AE1" s="3" t="s">
+      <c r="AE1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="AF1" s="3" t="s">
+      <c r="AF1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="AG1" s="3" t="s">
+      <c r="AG1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AH1" s="3" t="s">
+      <c r="AH1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="AI1" s="3" t="s">
+      <c r="AI1" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="AJ1" s="3" t="s">
+      <c r="AJ1" s="4" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A2" s="3"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="4"/>
-      <c r="R2" s="4"/>
-      <c r="S2" s="4"/>
-      <c r="T2" s="4"/>
-      <c r="U2" s="4"/>
-      <c r="V2" s="3"/>
-      <c r="W2" s="4"/>
-      <c r="X2" s="4"/>
-      <c r="Y2" s="4"/>
-      <c r="Z2" s="4"/>
-      <c r="AA2" s="3"/>
-      <c r="AB2" s="3"/>
-      <c r="AC2" s="3"/>
-      <c r="AD2" s="3"/>
-      <c r="AE2" s="3"/>
-      <c r="AF2" s="3"/>
-      <c r="AG2" s="3"/>
-      <c r="AH2" s="3"/>
-      <c r="AI2" s="3"/>
-      <c r="AJ2" s="3"/>
+      <c r="A2" s="4"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="4"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="3"/>
+      <c r="AA2" s="4"/>
+      <c r="AB2" s="4"/>
+      <c r="AC2" s="4"/>
+      <c r="AD2" s="4"/>
+      <c r="AE2" s="4"/>
+      <c r="AF2" s="4"/>
+      <c r="AG2" s="4"/>
+      <c r="AH2" s="4"/>
+      <c r="AI2" s="4"/>
+      <c r="AJ2" s="4"/>
     </row>
     <row r="3" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>32</v>
@@ -801,7 +801,7 @@
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="F3" s="1">
         <v>21</v>
@@ -810,70 +810,70 @@
         <v>7</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="L3" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="S3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="T3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="U3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="V3" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="W3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="X3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="Y3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="Z3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="AA3" s="1" t="s">
+      <c r="AB3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC3" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="AB3" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AC3" s="1" t="s">
-        <v>37</v>
       </c>
       <c r="AD3" s="1"/>
       <c r="AE3" s="1">
@@ -881,17 +881,17 @@
       </c>
       <c r="AF3" s="1"/>
       <c r="AG3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AH3" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="AH3" s="1" t="s">
-        <v>39</v>
       </c>
       <c r="AI3" s="1"/>
       <c r="AJ3" s="1"/>
     </row>
     <row r="4" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>32</v>
@@ -899,7 +899,7 @@
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="F4" s="1">
         <v>97</v>
@@ -908,70 +908,70 @@
         <v>1</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="X4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA4" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="L4" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q4" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="R4" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="S4" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="T4" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="U4" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="V4" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="W4" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="X4" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="Y4" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="Z4" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="AA4" s="1" t="s">
+      <c r="AB4" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC4" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="AB4" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AC4" s="1" t="s">
-        <v>37</v>
       </c>
       <c r="AD4" s="1"/>
       <c r="AE4" s="1">
@@ -979,17 +979,17 @@
       </c>
       <c r="AF4" s="1"/>
       <c r="AG4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AH4" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="AH4" s="1" t="s">
-        <v>39</v>
       </c>
       <c r="AI4" s="1"/>
       <c r="AJ4" s="1"/>
     </row>
     <row r="5" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>32</v>
@@ -997,7 +997,7 @@
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1" t="s">
-        <v>33</v>
+        <v>57</v>
       </c>
       <c r="F5" s="1">
         <v>6</v>
@@ -1006,70 +1006,70 @@
         <v>2</v>
       </c>
       <c r="H5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="U5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="W5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="X5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA5" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="I5" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="O5" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="P5" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q5" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="R5" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="S5" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="T5" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="U5" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="V5" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="W5" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="X5" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="Y5" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="Z5" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="AA5" s="1" t="s">
+      <c r="AB5" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC5" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="AB5" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AC5" s="1" t="s">
-        <v>37</v>
       </c>
       <c r="AD5" s="1"/>
       <c r="AE5" s="1">
@@ -1077,17 +1077,17 @@
       </c>
       <c r="AF5" s="1"/>
       <c r="AG5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AH5" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="AH5" s="1" t="s">
-        <v>39</v>
       </c>
       <c r="AI5" s="1"/>
       <c r="AJ5" s="1"/>
     </row>
     <row r="6" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>32</v>
@@ -1095,7 +1095,7 @@
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1" t="s">
-        <v>33</v>
+        <v>57</v>
       </c>
       <c r="F6" s="1">
         <v>44</v>
@@ -1104,70 +1104,70 @@
         <v>2</v>
       </c>
       <c r="H6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="T6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="U6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="V6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="W6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="X6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA6" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="I6" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="O6" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="P6" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q6" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="R6" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="S6" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="T6" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="U6" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="V6" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="W6" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="X6" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="Y6" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="Z6" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="AA6" s="1" t="s">
+      <c r="AB6" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC6" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="AB6" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AC6" s="1" t="s">
-        <v>37</v>
       </c>
       <c r="AD6" s="1"/>
       <c r="AE6" s="1">
@@ -1175,17 +1175,17 @@
       </c>
       <c r="AF6" s="1"/>
       <c r="AG6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AH6" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="AH6" s="1" t="s">
-        <v>39</v>
       </c>
       <c r="AI6" s="1"/>
       <c r="AJ6" s="1"/>
     </row>
     <row r="7" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>32</v>
@@ -1193,7 +1193,7 @@
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1" t="s">
-        <v>33</v>
+        <v>57</v>
       </c>
       <c r="F7" s="1">
         <v>55</v>
@@ -1202,70 +1202,70 @@
         <v>3</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="T7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="U7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="V7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="W7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="X7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA7" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="L7" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="N7" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="O7" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="P7" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q7" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="R7" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="S7" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="T7" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="U7" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="V7" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="W7" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="X7" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="Y7" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="Z7" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="AA7" s="1" t="s">
+      <c r="AB7" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC7" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="AB7" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AC7" s="1" t="s">
-        <v>37</v>
       </c>
       <c r="AD7" s="1"/>
       <c r="AE7" s="1">
@@ -1273,20 +1273,20 @@
       </c>
       <c r="AF7" s="1"/>
       <c r="AG7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AH7" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="AH7" s="1" t="s">
-        <v>39</v>
       </c>
       <c r="AI7" s="1"/>
       <c r="AJ7" s="1"/>
     </row>
     <row r="8" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C8" s="1">
         <v>24.8</v>
@@ -1295,79 +1295,79 @@
         <v>24.8</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>33</v>
+        <v>57</v>
       </c>
       <c r="F8" s="1">
         <v>22</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="Q8" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="R8" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="S8" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="T8" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="U8" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="V8" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="W8" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="X8" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="Y8" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="Z8" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AA8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AB8" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC8" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="AB8" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AC8" s="1" t="s">
-        <v>37</v>
       </c>
       <c r="AD8" s="1"/>
       <c r="AE8" s="1">
@@ -1375,20 +1375,20 @@
       </c>
       <c r="AF8" s="1"/>
       <c r="AG8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AH8" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="AH8" s="1" t="s">
-        <v>39</v>
       </c>
       <c r="AI8" s="1"/>
       <c r="AJ8" s="1"/>
     </row>
     <row r="9" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C9" s="1">
         <v>18.18</v>
@@ -1397,7 +1397,7 @@
         <v>18.18</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="F9" s="1">
         <v>17</v>
@@ -1406,70 +1406,70 @@
         <v>3</v>
       </c>
       <c r="H9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="R9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="S9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="T9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="U9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="V9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="W9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="X9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA9" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="I9" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="L9" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="M9" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="N9" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="O9" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="P9" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q9" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="R9" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="S9" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="T9" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="U9" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="V9" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="W9" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="X9" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="Y9" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="Z9" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="AA9" s="1" t="s">
+      <c r="AB9" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC9" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="AB9" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AC9" s="1" t="s">
-        <v>37</v>
       </c>
       <c r="AD9" s="1"/>
       <c r="AE9" s="1">
@@ -1477,17 +1477,17 @@
       </c>
       <c r="AF9" s="1"/>
       <c r="AG9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AH9" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="AH9" s="1" t="s">
-        <v>39</v>
       </c>
       <c r="AI9" s="1"/>
       <c r="AJ9" s="1"/>
     </row>
     <row r="10" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>32</v>
@@ -1495,7 +1495,7 @@
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="F10" s="1">
         <v>57</v>
@@ -1504,70 +1504,70 @@
         <v>5</v>
       </c>
       <c r="H10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="R10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="S10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="T10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="U10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="V10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="W10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="X10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA10" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="I10" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="M10" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="N10" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="O10" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="P10" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q10" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="R10" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="S10" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="T10" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="U10" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="V10" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="W10" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="X10" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="Y10" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="Z10" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="AA10" s="1" t="s">
+      <c r="AB10" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC10" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="AB10" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AC10" s="1" t="s">
-        <v>37</v>
       </c>
       <c r="AD10" s="1"/>
       <c r="AE10" s="1">
@@ -1575,17 +1575,17 @@
       </c>
       <c r="AF10" s="1"/>
       <c r="AG10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AH10" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="AH10" s="1" t="s">
-        <v>39</v>
       </c>
       <c r="AI10" s="1"/>
       <c r="AJ10" s="1"/>
     </row>
     <row r="11" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>32</v>
@@ -1593,7 +1593,7 @@
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="F11" s="1">
         <v>9</v>
@@ -1602,70 +1602,70 @@
         <v>11</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="R11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="S11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="T11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="U11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="V11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="W11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="X11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA11" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="L11" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="M11" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="N11" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="O11" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="P11" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q11" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="R11" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="S11" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="T11" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="U11" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="V11" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="W11" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="X11" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="Y11" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="Z11" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="AA11" s="1" t="s">
+      <c r="AB11" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC11" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="AB11" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AC11" s="1" t="s">
-        <v>37</v>
       </c>
       <c r="AD11" s="1"/>
       <c r="AE11" s="1">
@@ -1673,17 +1673,17 @@
       </c>
       <c r="AF11" s="1"/>
       <c r="AG11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AH11" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="AH11" s="1" t="s">
-        <v>39</v>
       </c>
       <c r="AI11" s="1"/>
       <c r="AJ11" s="1"/>
     </row>
     <row r="12" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>32</v>
@@ -1691,7 +1691,7 @@
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="F12" s="1">
         <v>31</v>
@@ -1700,70 +1700,70 @@
         <v>12</v>
       </c>
       <c r="H12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="O12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="P12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="R12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="S12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="T12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="U12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="V12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="W12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="X12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA12" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="I12" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="L12" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="M12" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="N12" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="O12" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="P12" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q12" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="R12" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="S12" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="T12" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="U12" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="V12" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="W12" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="X12" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="Y12" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="Z12" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="AA12" s="1" t="s">
+      <c r="AB12" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC12" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="AB12" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AC12" s="1" t="s">
-        <v>37</v>
       </c>
       <c r="AD12" s="1"/>
       <c r="AE12" s="1">
@@ -1771,16 +1771,40 @@
       </c>
       <c r="AF12" s="1"/>
       <c r="AG12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AH12" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="AH12" s="1" t="s">
-        <v>39</v>
       </c>
       <c r="AI12" s="1"/>
       <c r="AJ12" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="36">
+    <mergeCell ref="AJ1:AJ2"/>
+    <mergeCell ref="Y1:Y2"/>
+    <mergeCell ref="Z1:Z2"/>
+    <mergeCell ref="AA1:AA2"/>
+    <mergeCell ref="AB1:AB2"/>
+    <mergeCell ref="AC1:AC2"/>
+    <mergeCell ref="AD1:AD2"/>
+    <mergeCell ref="AE1:AE2"/>
+    <mergeCell ref="AF1:AF2"/>
+    <mergeCell ref="AG1:AG2"/>
+    <mergeCell ref="AH1:AH2"/>
+    <mergeCell ref="AI1:AI2"/>
+    <mergeCell ref="X1:X2"/>
+    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="N1:N2"/>
+    <mergeCell ref="O1:O2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="Q1:Q2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="V1:V2"/>
+    <mergeCell ref="W1:W2"/>
     <mergeCell ref="L1:L2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
@@ -1793,30 +1817,6 @@
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="K1:K2"/>
-    <mergeCell ref="X1:X2"/>
-    <mergeCell ref="M1:M2"/>
-    <mergeCell ref="N1:N2"/>
-    <mergeCell ref="O1:O2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="Q1:Q2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="V1:V2"/>
-    <mergeCell ref="W1:W2"/>
-    <mergeCell ref="AJ1:AJ2"/>
-    <mergeCell ref="Y1:Y2"/>
-    <mergeCell ref="Z1:Z2"/>
-    <mergeCell ref="AA1:AA2"/>
-    <mergeCell ref="AB1:AB2"/>
-    <mergeCell ref="AC1:AC2"/>
-    <mergeCell ref="AD1:AD2"/>
-    <mergeCell ref="AE1:AE2"/>
-    <mergeCell ref="AF1:AF2"/>
-    <mergeCell ref="AG1:AG2"/>
-    <mergeCell ref="AH1:AH2"/>
-    <mergeCell ref="AI1:AI2"/>
   </mergeCells>
   <conditionalFormatting sqref="H3:U12">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">

</xml_diff>

<commit_message>
Bulk upload on patient_cid not patient_id
Signed-off-by: James Noss <jnoss@jhu.edu>
</commit_message>
<xml_diff>
--- a/biospecdb/apps/uploader/tests/data/meta_data.xlsx
+++ b/biospecdb/apps/uploader/tests/data/meta_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamienoss/repos/biospecdb-project/biospecdb/biospecdb/apps/uploader/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F9875CD-4871-FD4A-B7FF-1AFC548AB8E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EF5E606-F765-8E42-A969-C224E6B24884}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5820" yWindow="3700" windowWidth="15040" windowHeight="14400" xr2:uid="{6C67B765-75CA-5F42-88FE-D1F4BED05A15}"/>
   </bookViews>
@@ -38,9 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="59">
   <si>
-    <t>Patient ID</t>
-  </si>
-  <si>
     <t>RESULT RT-qPCR</t>
   </si>
   <si>
@@ -213,6 +210,9 @@
   </si>
   <si>
     <t>prefer not to state</t>
+  </si>
+  <si>
+    <t>Patient CID</t>
   </si>
 </sst>
 </file>
@@ -301,10 +301,10 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -635,7 +635,7 @@
   <dimension ref="A1:AJ12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -644,164 +644,164 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="R1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="S1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="T1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="U1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="V1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="W1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="X1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="Y1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="Z1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="AA1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="AB1" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="AA1" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="AB1" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="AC1" s="4" t="s">
+      <c r="AD1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="AD1" s="4" t="s">
+      <c r="AE1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="AE1" s="4" t="s">
+      <c r="AF1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="AF1" s="4" t="s">
+      <c r="AG1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="AG1" s="4" t="s">
+      <c r="AH1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="AH1" s="4" t="s">
+      <c r="AI1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="AI1" s="4" t="s">
+      <c r="AJ1" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="AJ1" s="4" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A2" s="4"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="4"/>
-      <c r="Q2" s="3"/>
-      <c r="R2" s="3"/>
-      <c r="S2" s="3"/>
-      <c r="T2" s="3"/>
-      <c r="U2" s="3"/>
-      <c r="V2" s="4"/>
-      <c r="W2" s="3"/>
-      <c r="X2" s="3"/>
-      <c r="Y2" s="3"/>
-      <c r="Z2" s="3"/>
-      <c r="AA2" s="4"/>
-      <c r="AB2" s="4"/>
-      <c r="AC2" s="4"/>
-      <c r="AD2" s="4"/>
-      <c r="AE2" s="4"/>
-      <c r="AF2" s="4"/>
-      <c r="AG2" s="4"/>
-      <c r="AH2" s="4"/>
-      <c r="AI2" s="4"/>
-      <c r="AJ2" s="4"/>
+      <c r="A2" s="3"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="4"/>
+      <c r="R2" s="4"/>
+      <c r="S2" s="4"/>
+      <c r="T2" s="4"/>
+      <c r="U2" s="4"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="4"/>
+      <c r="X2" s="4"/>
+      <c r="Y2" s="4"/>
+      <c r="Z2" s="4"/>
+      <c r="AA2" s="3"/>
+      <c r="AB2" s="3"/>
+      <c r="AC2" s="3"/>
+      <c r="AD2" s="3"/>
+      <c r="AE2" s="3"/>
+      <c r="AF2" s="3"/>
+      <c r="AG2" s="3"/>
+      <c r="AH2" s="3"/>
+      <c r="AI2" s="3"/>
+      <c r="AJ2" s="3"/>
     </row>
     <row r="3" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F3" s="1">
         <v>21</v>
@@ -810,70 +810,70 @@
         <v>7</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="L3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="S3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="T3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="U3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="V3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="W3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="X3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Y3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Z3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="AA3" s="1" t="s">
+      <c r="AB3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AC3" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="AB3" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AC3" s="1" t="s">
-        <v>36</v>
       </c>
       <c r="AD3" s="1"/>
       <c r="AE3" s="1">
@@ -881,25 +881,25 @@
       </c>
       <c r="AF3" s="1"/>
       <c r="AG3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH3" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="AH3" s="1" t="s">
-        <v>38</v>
       </c>
       <c r="AI3" s="1"/>
       <c r="AJ3" s="1"/>
     </row>
     <row r="4" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F4" s="1">
         <v>97</v>
@@ -908,70 +908,70 @@
         <v>1</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="X4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA4" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="L4" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q4" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="R4" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="S4" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="T4" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="U4" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="V4" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="W4" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="X4" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Y4" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Z4" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="AA4" s="1" t="s">
+      <c r="AB4" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AC4" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="AB4" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AC4" s="1" t="s">
-        <v>36</v>
       </c>
       <c r="AD4" s="1"/>
       <c r="AE4" s="1">
@@ -979,25 +979,25 @@
       </c>
       <c r="AF4" s="1"/>
       <c r="AG4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH4" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="AH4" s="1" t="s">
-        <v>38</v>
       </c>
       <c r="AI4" s="1"/>
       <c r="AJ4" s="1"/>
     </row>
     <row r="5" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F5" s="1">
         <v>6</v>
@@ -1006,70 +1006,70 @@
         <v>2</v>
       </c>
       <c r="H5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="U5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="W5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="X5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA5" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="I5" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="O5" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="P5" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q5" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="R5" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="S5" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="T5" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="U5" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="V5" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="W5" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="X5" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Y5" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Z5" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="AA5" s="1" t="s">
+      <c r="AB5" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AC5" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="AB5" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AC5" s="1" t="s">
-        <v>36</v>
       </c>
       <c r="AD5" s="1"/>
       <c r="AE5" s="1">
@@ -1077,25 +1077,25 @@
       </c>
       <c r="AF5" s="1"/>
       <c r="AG5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH5" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="AH5" s="1" t="s">
-        <v>38</v>
       </c>
       <c r="AI5" s="1"/>
       <c r="AJ5" s="1"/>
     </row>
     <row r="6" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F6" s="1">
         <v>44</v>
@@ -1104,70 +1104,70 @@
         <v>2</v>
       </c>
       <c r="H6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="T6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="U6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="V6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="W6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="X6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA6" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="I6" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="O6" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="P6" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q6" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="R6" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="S6" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="T6" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="U6" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="V6" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="W6" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="X6" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Y6" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Z6" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="AA6" s="1" t="s">
+      <c r="AB6" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AC6" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="AB6" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AC6" s="1" t="s">
-        <v>36</v>
       </c>
       <c r="AD6" s="1"/>
       <c r="AE6" s="1">
@@ -1175,25 +1175,25 @@
       </c>
       <c r="AF6" s="1"/>
       <c r="AG6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH6" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="AH6" s="1" t="s">
-        <v>38</v>
       </c>
       <c r="AI6" s="1"/>
       <c r="AJ6" s="1"/>
     </row>
     <row r="7" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F7" s="1">
         <v>55</v>
@@ -1202,70 +1202,70 @@
         <v>3</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="T7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="U7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="V7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="W7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="X7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA7" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="L7" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="N7" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="O7" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="P7" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q7" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="R7" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="S7" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="T7" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="U7" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="V7" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="W7" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="X7" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Y7" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Z7" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="AA7" s="1" t="s">
+      <c r="AB7" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AC7" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="AB7" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AC7" s="1" t="s">
-        <v>36</v>
       </c>
       <c r="AD7" s="1"/>
       <c r="AE7" s="1">
@@ -1273,20 +1273,20 @@
       </c>
       <c r="AF7" s="1"/>
       <c r="AG7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH7" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="AH7" s="1" t="s">
-        <v>38</v>
       </c>
       <c r="AI7" s="1"/>
       <c r="AJ7" s="1"/>
     </row>
     <row r="8" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C8" s="1">
         <v>24.8</v>
@@ -1295,79 +1295,79 @@
         <v>24.8</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F8" s="1">
         <v>22</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="Q8" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="R8" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="S8" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="T8" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="U8" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="V8" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="W8" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="X8" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="Y8" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="Z8" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AA8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB8" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AC8" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="AB8" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AC8" s="1" t="s">
-        <v>36</v>
       </c>
       <c r="AD8" s="1"/>
       <c r="AE8" s="1">
@@ -1375,20 +1375,20 @@
       </c>
       <c r="AF8" s="1"/>
       <c r="AG8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH8" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="AH8" s="1" t="s">
-        <v>38</v>
       </c>
       <c r="AI8" s="1"/>
       <c r="AJ8" s="1"/>
     </row>
     <row r="9" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C9" s="1">
         <v>18.18</v>
@@ -1397,7 +1397,7 @@
         <v>18.18</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F9" s="1">
         <v>17</v>
@@ -1406,70 +1406,70 @@
         <v>3</v>
       </c>
       <c r="H9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="R9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="S9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="T9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="U9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="V9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="W9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="X9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA9" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="I9" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="L9" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="M9" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="N9" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="O9" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="P9" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q9" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="R9" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="S9" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="T9" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="U9" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="V9" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="W9" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="X9" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Y9" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Z9" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="AA9" s="1" t="s">
+      <c r="AB9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AC9" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="AB9" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AC9" s="1" t="s">
-        <v>36</v>
       </c>
       <c r="AD9" s="1"/>
       <c r="AE9" s="1">
@@ -1477,25 +1477,25 @@
       </c>
       <c r="AF9" s="1"/>
       <c r="AG9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH9" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="AH9" s="1" t="s">
-        <v>38</v>
       </c>
       <c r="AI9" s="1"/>
       <c r="AJ9" s="1"/>
     </row>
     <row r="10" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F10" s="1">
         <v>57</v>
@@ -1504,70 +1504,70 @@
         <v>5</v>
       </c>
       <c r="H10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="R10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="S10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="T10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="U10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="V10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="W10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="X10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA10" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="I10" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="M10" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="N10" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="O10" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="P10" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q10" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="R10" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="S10" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="T10" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="U10" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="V10" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="W10" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="X10" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Y10" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Z10" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="AA10" s="1" t="s">
+      <c r="AB10" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AC10" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="AB10" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AC10" s="1" t="s">
-        <v>36</v>
       </c>
       <c r="AD10" s="1"/>
       <c r="AE10" s="1">
@@ -1575,25 +1575,25 @@
       </c>
       <c r="AF10" s="1"/>
       <c r="AG10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH10" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="AH10" s="1" t="s">
-        <v>38</v>
       </c>
       <c r="AI10" s="1"/>
       <c r="AJ10" s="1"/>
     </row>
     <row r="11" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F11" s="1">
         <v>9</v>
@@ -1602,70 +1602,70 @@
         <v>11</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="R11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="S11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="T11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="U11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="V11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="W11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="X11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA11" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="L11" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="M11" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="N11" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="O11" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="P11" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q11" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="R11" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="S11" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="T11" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="U11" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="V11" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="W11" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="X11" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Y11" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Z11" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="AA11" s="1" t="s">
+      <c r="AB11" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AC11" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="AB11" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AC11" s="1" t="s">
-        <v>36</v>
       </c>
       <c r="AD11" s="1"/>
       <c r="AE11" s="1">
@@ -1673,25 +1673,25 @@
       </c>
       <c r="AF11" s="1"/>
       <c r="AG11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH11" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="AH11" s="1" t="s">
-        <v>38</v>
       </c>
       <c r="AI11" s="1"/>
       <c r="AJ11" s="1"/>
     </row>
     <row r="12" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F12" s="1">
         <v>31</v>
@@ -1700,70 +1700,70 @@
         <v>12</v>
       </c>
       <c r="H12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="P12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="R12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="S12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="T12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="U12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="V12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="W12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="X12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA12" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="I12" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="L12" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="M12" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="N12" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="O12" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="P12" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q12" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="R12" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="S12" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="T12" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="U12" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="V12" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="W12" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="X12" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Y12" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Z12" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="AA12" s="1" t="s">
+      <c r="AB12" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AC12" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="AB12" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AC12" s="1" t="s">
-        <v>36</v>
       </c>
       <c r="AD12" s="1"/>
       <c r="AE12" s="1">
@@ -1771,16 +1771,40 @@
       </c>
       <c r="AF12" s="1"/>
       <c r="AG12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH12" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="AH12" s="1" t="s">
-        <v>38</v>
       </c>
       <c r="AI12" s="1"/>
       <c r="AJ12" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="36">
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="X1:X2"/>
+    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="N1:N2"/>
+    <mergeCell ref="O1:O2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="Q1:Q2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="V1:V2"/>
+    <mergeCell ref="W1:W2"/>
     <mergeCell ref="AJ1:AJ2"/>
     <mergeCell ref="Y1:Y2"/>
     <mergeCell ref="Z1:Z2"/>
@@ -1793,30 +1817,6 @@
     <mergeCell ref="AG1:AG2"/>
     <mergeCell ref="AH1:AH2"/>
     <mergeCell ref="AI1:AI2"/>
-    <mergeCell ref="X1:X2"/>
-    <mergeCell ref="M1:M2"/>
-    <mergeCell ref="N1:N2"/>
-    <mergeCell ref="O1:O2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="Q1:Q2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="V1:V2"/>
-    <mergeCell ref="W1:W2"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="J1:J2"/>
-    <mergeCell ref="K1:K2"/>
   </mergeCells>
   <conditionalFormatting sqref="H3:U12">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">

</xml_diff>